<commit_message>
Added okadaic acid to the analysis
</commit_message>
<xml_diff>
--- a/haddock.xlsx
+++ b/haddock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\istva\projects\research\docking_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858F3C17-175D-463D-9E59-140FC1D8745C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3DB563-B382-4707-BB7B-DC691A838B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3F3DB53-D8DC-4E44-8758-43014728F58F}"/>
   </bookViews>
@@ -458,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB14277-D2C8-4B08-BAA5-8CAA37C0C43A}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="A14:O14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,6 +1235,241 @@
         <v>-0.6</v>
       </c>
     </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-59</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0.7</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>-24.4</v>
+      </c>
+      <c r="F17">
+        <v>13.2</v>
+      </c>
+      <c r="G17">
+        <v>-335.3</v>
+      </c>
+      <c r="H17">
+        <v>26.1</v>
+      </c>
+      <c r="I17">
+        <v>-13.4</v>
+      </c>
+      <c r="J17">
+        <v>1.9</v>
+      </c>
+      <c r="K17">
+        <v>123.5</v>
+      </c>
+      <c r="L17">
+        <v>35.75</v>
+      </c>
+      <c r="M17">
+        <v>1234.8</v>
+      </c>
+      <c r="N17">
+        <v>11.5</v>
+      </c>
+      <c r="O17">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-57.5</v>
+      </c>
+      <c r="B18">
+        <v>9.5</v>
+      </c>
+      <c r="C18">
+        <v>0.7</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>-22.7</v>
+      </c>
+      <c r="F18">
+        <v>10.3</v>
+      </c>
+      <c r="G18">
+        <v>-338.3</v>
+      </c>
+      <c r="H18">
+        <v>22.8</v>
+      </c>
+      <c r="I18">
+        <v>-13.3</v>
+      </c>
+      <c r="J18">
+        <v>1.8</v>
+      </c>
+      <c r="K18">
+        <v>123.1</v>
+      </c>
+      <c r="L18">
+        <v>35.590000000000003</v>
+      </c>
+      <c r="M18">
+        <v>1237.5999999999999</v>
+      </c>
+      <c r="N18">
+        <v>11.7</v>
+      </c>
+      <c r="O18">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-64.3</v>
+      </c>
+      <c r="B19">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C19">
+        <v>0.2</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="E19">
+        <v>-24.7</v>
+      </c>
+      <c r="F19">
+        <v>6.3</v>
+      </c>
+      <c r="G19">
+        <v>-392.5</v>
+      </c>
+      <c r="H19">
+        <v>48.5</v>
+      </c>
+      <c r="I19">
+        <v>-12.6</v>
+      </c>
+      <c r="J19">
+        <v>0.3</v>
+      </c>
+      <c r="K19">
+        <v>121.7</v>
+      </c>
+      <c r="L19">
+        <v>42.94</v>
+      </c>
+      <c r="M19">
+        <v>1205.5</v>
+      </c>
+      <c r="N19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="O19">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-65.8</v>
+      </c>
+      <c r="B20">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C20">
+        <v>0.7</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+      <c r="E20">
+        <v>-29.7</v>
+      </c>
+      <c r="F20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G20">
+        <v>-363.8</v>
+      </c>
+      <c r="H20">
+        <v>45.5</v>
+      </c>
+      <c r="I20">
+        <v>-12.8</v>
+      </c>
+      <c r="J20">
+        <v>0.8</v>
+      </c>
+      <c r="K20">
+        <v>130.1</v>
+      </c>
+      <c r="L20">
+        <v>30.73</v>
+      </c>
+      <c r="M20">
+        <v>1212</v>
+      </c>
+      <c r="N20">
+        <v>5</v>
+      </c>
+      <c r="O20">
+        <v>-1.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-72.900000000000006</v>
+      </c>
+      <c r="B21">
+        <v>10.9</v>
+      </c>
+      <c r="C21">
+        <v>0.7</v>
+      </c>
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+      <c r="E21">
+        <v>-34.4</v>
+      </c>
+      <c r="F21">
+        <v>11.3</v>
+      </c>
+      <c r="G21">
+        <v>-340.5</v>
+      </c>
+      <c r="H21">
+        <v>39.6</v>
+      </c>
+      <c r="I21">
+        <v>-14.8</v>
+      </c>
+      <c r="J21">
+        <v>1.4</v>
+      </c>
+      <c r="K21">
+        <v>104.6</v>
+      </c>
+      <c r="L21">
+        <v>21.86</v>
+      </c>
+      <c r="M21">
+        <v>1224</v>
+      </c>
+      <c r="N21">
+        <v>6.9</v>
+      </c>
+      <c r="O21">
+        <v>-2.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>